<commit_message>
Modify truncated normal distribution
</commit_message>
<xml_diff>
--- a/U.xlsx
+++ b/U.xlsx
@@ -1,34 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Programming\Python\ToleranceAndRate\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D077D9-3457-4FB5-8C3E-1C2D38F852E2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>noinspect_U</t>
   </si>
@@ -47,15 +33,12 @@
   <si>
     <t>inspect_Up</t>
   </si>
-  <si>
-    <t>error</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,7 +63,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -103,27 +86,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -132,14 +101,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -186,7 +147,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -218,27 +179,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -270,24 +213,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -463,25 +388,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="8" width="12" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -489,345 +403,316 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
-        <v>4.0038078550661123</v>
+        <v>3.68130764554671</v>
       </c>
       <c r="B2">
-        <v>4.0540710441061769</v>
+        <v>3.712880264770847</v>
       </c>
       <c r="C2">
-        <f>(A2-B2)/B2</f>
-        <v>-1.2398201337181169E-2</v>
+        <v>3.691249946667718</v>
       </c>
       <c r="D2">
-        <v>4.0145881448697827</v>
+        <v>3.710590627448494</v>
       </c>
       <c r="E2">
-        <v>4.0426075652044497</v>
+        <v>3.680695898027637</v>
       </c>
       <c r="F2">
-        <f>(D2-E2)/E2</f>
-        <v>-6.9310265423327185E-3</v>
-      </c>
-      <c r="G2">
-        <v>3.9930512627859218</v>
-      </c>
-      <c r="H2">
-        <v>4.0352964026423397</v>
-      </c>
-      <c r="I2">
-        <f>(G2-H2)/H2</f>
-        <v>-1.046890628127229E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3.709446122143752</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
-        <v>4.0974502278539413</v>
+        <v>3.778910672287936</v>
       </c>
       <c r="B3">
-        <v>4.1451383275740792</v>
+        <v>3.816692314724387</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C11" si="0">(A3-B3)/B3</f>
-        <v>-1.15045858428679E-2</v>
+        <v>3.789108209787422</v>
       </c>
       <c r="D3">
-        <v>4.1084713821058196</v>
+        <v>3.814052323365775</v>
       </c>
       <c r="E3">
-        <v>4.1359442409187297</v>
+        <v>3.776795825073335</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F11" si="1">(D3-E3)/E3</f>
-        <v>-6.6424635373728913E-3</v>
-      </c>
-      <c r="G3">
-        <v>4.0797320538111599</v>
-      </c>
-      <c r="H3">
-        <v>4.1265968602658019</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I11" si="2">(G3-H3)/H3</f>
-        <v>-1.1356768795588945E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3.811870961153208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
-        <v>4.1992586903083007</v>
+        <v>3.895553760348336</v>
       </c>
       <c r="B4">
-        <v>4.2475944326700938</v>
+        <v>3.940694378439463</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
-        <v>-1.1379556859294752E-2</v>
+        <v>3.90605438561461</v>
       </c>
       <c r="D4">
-        <v>4.2105407975924312</v>
+        <v>3.935471151286984</v>
       </c>
       <c r="E4">
-        <v>4.2364279105203364</v>
+        <v>3.889414484574714</v>
       </c>
       <c r="F4">
-        <f t="shared" si="1"/>
-        <v>-6.1105991827736959E-3</v>
-      </c>
-      <c r="G4">
-        <v>4.1693016997209398</v>
-      </c>
-      <c r="H4">
-        <v>4.2262804793017832</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="2"/>
-        <v>-1.3482015654166138E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3.928180919567278</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
-        <v>4.3089294989873466</v>
+        <v>4.033005854684299</v>
       </c>
       <c r="B5">
-        <v>4.3551087924942617</v>
+        <v>4.075944709271789</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
-        <v>-1.0603476447362717E-2</v>
+        <v>4.043861342889096</v>
       </c>
       <c r="D5">
-        <v>4.3204918337156064</v>
+        <v>4.067441030686422</v>
       </c>
       <c r="E5">
-        <v>4.3616658757103677</v>
+        <v>4.018112310043471</v>
       </c>
       <c r="F5">
-        <f t="shared" si="1"/>
-        <v>-9.4399807706626333E-3</v>
-      </c>
-      <c r="G5">
-        <v>4.2592388091509719</v>
-      </c>
-      <c r="H5">
-        <v>4.3232013768254429</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="2"/>
-        <v>-1.4795185812380367E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4.059387621258743</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
-        <v>4.4260037433639754</v>
+        <v>4.191721313010837</v>
       </c>
       <c r="B6">
-        <v>4.4824848766399823</v>
+        <v>4.231855686418858</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
-        <v>-1.2600406879307642E-2</v>
+        <v>4.202984129610075</v>
       </c>
       <c r="D6">
-        <v>4.4378644071836844</v>
+        <v>4.230908641358964</v>
       </c>
       <c r="E6">
-        <v>4.4627974630207996</v>
+        <v>4.161084907770253</v>
       </c>
       <c r="F6">
-        <f t="shared" si="1"/>
-        <v>-5.586866991772116E-3</v>
-      </c>
-      <c r="G6">
-        <v>4.3482932781185069</v>
-      </c>
-      <c r="H6">
-        <v>4.4409444363771637</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="2"/>
-        <v>-2.0862940211483463E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4.213482205822723</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
-        <v>4.5499198073483686</v>
+        <v>4.370761123810461</v>
       </c>
       <c r="B7">
-        <v>4.6004122144143063</v>
+        <v>4.41741108416563</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
-        <v>-1.0975626685741674E-2</v>
+        <v>4.382481112081479</v>
       </c>
       <c r="D7">
-        <v>4.5620954961127982</v>
+        <v>4.397327952269572</v>
       </c>
       <c r="E7">
-        <v>4.5870306330604453</v>
+        <v>4.315887549929587</v>
       </c>
       <c r="F7">
-        <f t="shared" si="1"/>
-        <v>-5.4360083771689454E-3</v>
-      </c>
-      <c r="G7">
-        <v>4.4360322108385448</v>
-      </c>
-      <c r="H7">
-        <v>4.5596134415384144</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="2"/>
-        <v>-2.7103444685471684E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4.384328549032622</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
-        <v>4.6800636985374604</v>
+        <v>4.568145119818779</v>
       </c>
       <c r="B8">
-        <v>4.7559349539369524</v>
+        <v>4.620962661166881</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
-        <v>-1.5952963220551612E-2</v>
+        <v>4.580367087031669</v>
       </c>
       <c r="D8">
-        <v>4.6925695877751528</v>
+        <v>4.601634834011843</v>
       </c>
       <c r="E8">
-        <v>4.7090690443286674</v>
+        <v>4.480087788066876</v>
       </c>
       <c r="F8">
-        <f t="shared" si="1"/>
-        <v>-3.5037618684707096E-3</v>
-      </c>
-      <c r="G8">
-        <v>4.5220454309415272</v>
-      </c>
-      <c r="H8">
-        <v>4.6879543888795094</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="2"/>
-        <v>-3.5390480404745774E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4.551263547975063</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
-        <v>4.8158102841080961</v>
+        <v>4.781382085715231</v>
       </c>
       <c r="B9">
-        <v>4.858544057748742</v>
+        <v>4.823387120895568</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
-        <v>-8.7955924928767755E-3</v>
+        <v>4.79414465741933</v>
       </c>
       <c r="D9">
-        <v>4.828660011015228</v>
+        <v>4.805587766296322</v>
       </c>
       <c r="E9">
-        <v>4.8362903765043059</v>
+        <v>4.651589544758843</v>
       </c>
       <c r="F9">
-        <f t="shared" si="1"/>
-        <v>-1.5777310490180249E-3</v>
-      </c>
-      <c r="G9">
-        <v>4.6059312802795702</v>
-      </c>
-      <c r="H9">
-        <v>4.8090323954818919</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="2"/>
-        <v>-4.2233259936684163E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4.726365843226637</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
-        <v>4.9565530052173692</v>
+        <v>5.007919295906796</v>
       </c>
       <c r="B10">
-        <v>5.0093652218477773</v>
+        <v>5.054220764034276</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
-        <v>-1.0542696387972204E-2</v>
+        <v>5.021254824515045</v>
       </c>
       <c r="D10">
-        <v>4.9697587196313746</v>
+        <v>5.03147176881349</v>
       </c>
       <c r="E10">
-        <v>4.9958353863354361</v>
+        <v>4.828708878425948</v>
       </c>
       <c r="F10">
-        <f t="shared" si="1"/>
-        <v>-5.21968093171888E-3</v>
-      </c>
-      <c r="G10">
-        <v>4.6875757566331302</v>
-      </c>
-      <c r="H10">
-        <v>4.9337177931042326</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="2"/>
-        <v>-4.9889768080195157E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4.929985479087242</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
-        <v>5.1017227342190106</v>
+        <v>5.245412014330283</v>
       </c>
       <c r="B11">
-        <v>5.1534441167804186</v>
+        <v>5.288023866335534</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
-        <v>-1.0036275040413288E-2</v>
+        <v>5.259347113282382</v>
       </c>
       <c r="D11">
-        <v>5.1152951931764674</v>
+        <v>5.272058502355177</v>
       </c>
       <c r="E11">
-        <v>5.1442594171918348</v>
+        <v>5.010136260825527</v>
       </c>
       <c r="F11">
-        <f t="shared" si="1"/>
-        <v>-5.6303972382439537E-3</v>
-      </c>
-      <c r="G11">
-        <v>4.7671024521225371</v>
-      </c>
-      <c r="H11">
-        <v>5.0904308680354369</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="2"/>
-        <v>-6.3516905404450111E-2</v>
+        <v>5.11618013293284</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>5.491836630314497</v>
+      </c>
+      <c r="B12">
+        <v>5.560884995391283</v>
+      </c>
+      <c r="C12">
+        <v>5.506392967659994</v>
+      </c>
+      <c r="D12">
+        <v>5.510181495362578</v>
+      </c>
+      <c r="E12">
+        <v>5.19486642250255</v>
+      </c>
+      <c r="F12">
+        <v>5.305371671880438</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>5.745507554150859</v>
+      </c>
+      <c r="B13">
+        <v>5.791103104852461</v>
+      </c>
+      <c r="C13">
+        <v>5.76070268050018</v>
+      </c>
+      <c r="D13">
+        <v>5.767806357316401</v>
+      </c>
+      <c r="E13">
+        <v>5.382129703277321</v>
+      </c>
+      <c r="F13">
+        <v>5.522997091854795</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>6.005047739561918</v>
+      </c>
+      <c r="B14">
+        <v>6.02550408465936</v>
+      </c>
+      <c r="C14">
+        <v>6.020895841900298</v>
+      </c>
+      <c r="D14">
+        <v>6.013110997212555</v>
+      </c>
+      <c r="E14">
+        <v>5.571335290317016</v>
+      </c>
+      <c r="F14">
+        <v>5.718959794584615</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>6.269342964479336</v>
+      </c>
+      <c r="B15">
+        <v>6.295343428837627</v>
+      </c>
+      <c r="C15">
+        <v>6.285855507963042</v>
+      </c>
+      <c r="D15">
+        <v>6.258591038420454</v>
+      </c>
+      <c r="E15">
+        <v>5.762027277637221</v>
+      </c>
+      <c r="F15">
+        <v>5.930929702529274</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>6.537494920499659</v>
+      </c>
+      <c r="B16">
+        <v>6.568324003439976</v>
+      </c>
+      <c r="C16">
+        <v>6.554681175985243</v>
+      </c>
+      <c r="D16">
+        <v>6.537085833282636</v>
+      </c>
+      <c r="E16">
+        <v>5.953851609744802</v>
+      </c>
+      <c r="F16">
+        <v>6.134261711623411</v>
       </c>
     </row>
   </sheetData>

</xml_diff>